<commit_message>
reset to latest model version config
</commit_message>
<xml_diff>
--- a/run_cloud_experiments/input/300_gridConnections/db_backboneConfig_300.xlsx
+++ b/run_cloud_experiments/input/300_gridConnections/db_backboneConfig_300.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\run_cloud_experiments\input\300_gridConnections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\WIES4\Documents\00projecten\HOLON\HOLON-anylogic\run_cloud_experiments\input\300_gridConnections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A514FB7F-523F-48FE-9A2A-E60BE633D5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB80B11B-6EE0-4AA3-8AB1-9CB33884B249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -2153,12 +2153,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12656,7 +12655,7 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -12673,7 +12672,7 @@
       <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12690,7 +12689,7 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12707,7 +12706,7 @@
       <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12724,7 +12723,7 @@
       <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12741,7 +12740,7 @@
       <c r="D6" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12758,7 +12757,7 @@
       <c r="D7" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12775,7 +12774,7 @@
       <c r="D8" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12792,7 +12791,7 @@
       <c r="D9" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12809,7 +12808,7 @@
       <c r="D10" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12826,7 +12825,7 @@
       <c r="D11" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12843,7 +12842,7 @@
       <c r="D12" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12860,7 +12859,7 @@
       <c r="D13" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12877,7 +12876,7 @@
       <c r="D14" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12894,7 +12893,7 @@
       <c r="D15" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12911,7 +12910,7 @@
       <c r="D16" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12928,7 +12927,7 @@
       <c r="D17" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12945,7 +12944,7 @@
       <c r="D18" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12962,7 +12961,7 @@
       <c r="D19" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12979,7 +12978,7 @@
       <c r="D20" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12996,7 +12995,7 @@
       <c r="D21" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13013,7 +13012,7 @@
       <c r="D22" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" t="s">
         <v>97</v>
       </c>
     </row>
@@ -13030,7 +13029,7 @@
       <c r="D23" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" t="s">
         <v>97</v>
       </c>
     </row>
@@ -13047,7 +13046,7 @@
       <c r="D24" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" t="s">
         <v>92</v>
       </c>
     </row>
@@ -13064,7 +13063,7 @@
       <c r="D25" t="s">
         <v>643</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13081,7 +13080,7 @@
       <c r="D26" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13098,7 +13097,7 @@
       <c r="D27" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13115,7 +13114,7 @@
       <c r="D28" t="s">
         <v>106</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13132,7 +13131,7 @@
       <c r="D29" t="s">
         <v>107</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13149,7 +13148,7 @@
       <c r="D30" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13166,7 +13165,7 @@
       <c r="D31" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13183,7 +13182,7 @@
       <c r="D32" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13200,7 +13199,7 @@
       <c r="D33" t="s">
         <v>111</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13217,7 +13216,7 @@
       <c r="D34" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13234,7 +13233,7 @@
       <c r="D35" t="s">
         <v>113</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13251,7 +13250,7 @@
       <c r="D36" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13268,7 +13267,7 @@
       <c r="D37" t="s">
         <v>115</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13285,7 +13284,7 @@
       <c r="D38" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13302,7 +13301,7 @@
       <c r="D39" t="s">
         <v>117</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13319,7 +13318,7 @@
       <c r="D40" t="s">
         <v>118</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13336,7 +13335,7 @@
       <c r="D41" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13353,7 +13352,7 @@
       <c r="D42" t="s">
         <v>120</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13370,7 +13369,7 @@
       <c r="D43" t="s">
         <v>121</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13387,7 +13386,7 @@
       <c r="D44" t="s">
         <v>122</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13404,7 +13403,7 @@
       <c r="D45" t="s">
         <v>123</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13421,7 +13420,7 @@
       <c r="D46" t="s">
         <v>124</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13438,7 +13437,7 @@
       <c r="D47" t="s">
         <v>125</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13455,7 +13454,7 @@
       <c r="D48" t="s">
         <v>126</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13472,7 +13471,7 @@
       <c r="D49" t="s">
         <v>127</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13489,7 +13488,7 @@
       <c r="D50" t="s">
         <v>128</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13506,7 +13505,7 @@
       <c r="D51" t="s">
         <v>129</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13523,7 +13522,7 @@
       <c r="D52" t="s">
         <v>130</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13540,7 +13539,7 @@
       <c r="D53" t="s">
         <v>131</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13557,7 +13556,7 @@
       <c r="D54" t="s">
         <v>132</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13574,7 +13573,7 @@
       <c r="D55" t="s">
         <v>133</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13591,7 +13590,7 @@
       <c r="D56" t="s">
         <v>134</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13608,7 +13607,7 @@
       <c r="D57" t="s">
         <v>135</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13625,7 +13624,7 @@
       <c r="D58" t="s">
         <v>136</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13642,7 +13641,7 @@
       <c r="D59" t="s">
         <v>137</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13659,7 +13658,7 @@
       <c r="D60" t="s">
         <v>138</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13676,7 +13675,7 @@
       <c r="D61" t="s">
         <v>139</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13693,7 +13692,7 @@
       <c r="D62" t="s">
         <v>140</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13710,7 +13709,7 @@
       <c r="D63" t="s">
         <v>141</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13727,7 +13726,7 @@
       <c r="D64" t="s">
         <v>142</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13744,7 +13743,7 @@
       <c r="D65" t="s">
         <v>143</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13761,7 +13760,7 @@
       <c r="D66" t="s">
         <v>144</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13778,7 +13777,7 @@
       <c r="D67" t="s">
         <v>145</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13795,7 +13794,7 @@
       <c r="D68" t="s">
         <v>146</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13812,7 +13811,7 @@
       <c r="D69" t="s">
         <v>147</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13829,7 +13828,7 @@
       <c r="D70" t="s">
         <v>148</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13846,7 +13845,7 @@
       <c r="D71" t="s">
         <v>149</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13863,7 +13862,7 @@
       <c r="D72" t="s">
         <v>150</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13880,7 +13879,7 @@
       <c r="D73" t="s">
         <v>151</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13897,7 +13896,7 @@
       <c r="D74" t="s">
         <v>152</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13914,7 +13913,7 @@
       <c r="D75" t="s">
         <v>153</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="E75" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13931,7 +13930,7 @@
       <c r="D76" t="s">
         <v>154</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E76" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13948,7 +13947,7 @@
       <c r="D77" t="s">
         <v>155</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E77" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13965,7 +13964,7 @@
       <c r="D78" t="s">
         <v>156</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13982,7 +13981,7 @@
       <c r="D79" t="s">
         <v>157</v>
       </c>
-      <c r="E79" s="4" t="s">
+      <c r="E79" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13999,7 +13998,7 @@
       <c r="D80" t="s">
         <v>158</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E80" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14016,7 +14015,7 @@
       <c r="D81" t="s">
         <v>159</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14033,7 +14032,7 @@
       <c r="D82" t="s">
         <v>160</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E82" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14050,7 +14049,7 @@
       <c r="D83" t="s">
         <v>161</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E83" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14067,7 +14066,7 @@
       <c r="D84" t="s">
         <v>162</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E84" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14084,7 +14083,7 @@
       <c r="D85" t="s">
         <v>163</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14101,7 +14100,7 @@
       <c r="D86" t="s">
         <v>164</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14118,7 +14117,7 @@
       <c r="D87" t="s">
         <v>165</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E87" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14135,7 +14134,7 @@
       <c r="D88" t="s">
         <v>166</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E88" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14152,7 +14151,7 @@
       <c r="D89" t="s">
         <v>167</v>
       </c>
-      <c r="E89" s="4" t="s">
+      <c r="E89" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14169,7 +14168,7 @@
       <c r="D90" t="s">
         <v>168</v>
       </c>
-      <c r="E90" s="4" t="s">
+      <c r="E90" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14186,7 +14185,7 @@
       <c r="D91" t="s">
         <v>169</v>
       </c>
-      <c r="E91" s="4" t="s">
+      <c r="E91" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14203,7 +14202,7 @@
       <c r="D92" t="s">
         <v>170</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="E92" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14220,7 +14219,7 @@
       <c r="D93" t="s">
         <v>171</v>
       </c>
-      <c r="E93" s="4" t="s">
+      <c r="E93" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14237,7 +14236,7 @@
       <c r="D94" t="s">
         <v>172</v>
       </c>
-      <c r="E94" s="4" t="s">
+      <c r="E94" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14254,7 +14253,7 @@
       <c r="D95" t="s">
         <v>173</v>
       </c>
-      <c r="E95" s="4" t="s">
+      <c r="E95" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14271,7 +14270,7 @@
       <c r="D96" t="s">
         <v>174</v>
       </c>
-      <c r="E96" s="4" t="s">
+      <c r="E96" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14288,7 +14287,7 @@
       <c r="D97" t="s">
         <v>175</v>
       </c>
-      <c r="E97" s="4" t="s">
+      <c r="E97" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14305,7 +14304,7 @@
       <c r="D98" t="s">
         <v>176</v>
       </c>
-      <c r="E98" s="4" t="s">
+      <c r="E98" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14322,7 +14321,7 @@
       <c r="D99" t="s">
         <v>177</v>
       </c>
-      <c r="E99" s="4" t="s">
+      <c r="E99" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14339,7 +14338,7 @@
       <c r="D100" t="s">
         <v>178</v>
       </c>
-      <c r="E100" s="4" t="s">
+      <c r="E100" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14356,7 +14355,7 @@
       <c r="D101" t="s">
         <v>179</v>
       </c>
-      <c r="E101" s="4" t="s">
+      <c r="E101" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14373,7 +14372,7 @@
       <c r="D102" t="s">
         <v>180</v>
       </c>
-      <c r="E102" s="4" t="s">
+      <c r="E102" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14390,7 +14389,7 @@
       <c r="D103" t="s">
         <v>181</v>
       </c>
-      <c r="E103" s="4" t="s">
+      <c r="E103" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14407,7 +14406,7 @@
       <c r="D104" t="s">
         <v>182</v>
       </c>
-      <c r="E104" s="4" t="s">
+      <c r="E104" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14424,7 +14423,7 @@
       <c r="D105" t="s">
         <v>183</v>
       </c>
-      <c r="E105" s="4" t="s">
+      <c r="E105" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14441,7 +14440,7 @@
       <c r="D106" t="s">
         <v>184</v>
       </c>
-      <c r="E106" s="4" t="s">
+      <c r="E106" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14458,7 +14457,7 @@
       <c r="D107" t="s">
         <v>185</v>
       </c>
-      <c r="E107" s="4" t="s">
+      <c r="E107" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14475,7 +14474,7 @@
       <c r="D108" t="s">
         <v>268</v>
       </c>
-      <c r="E108" s="4" t="s">
+      <c r="E108" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14492,7 +14491,7 @@
       <c r="D109" t="s">
         <v>270</v>
       </c>
-      <c r="E109" s="4" t="s">
+      <c r="E109" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14509,7 +14508,7 @@
       <c r="D110" t="s">
         <v>271</v>
       </c>
-      <c r="E110" s="4" t="s">
+      <c r="E110" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14526,7 +14525,7 @@
       <c r="D111" t="s">
         <v>272</v>
       </c>
-      <c r="E111" s="4" t="s">
+      <c r="E111" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14543,7 +14542,7 @@
       <c r="D112" t="s">
         <v>273</v>
       </c>
-      <c r="E112" s="4" t="s">
+      <c r="E112" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14560,7 +14559,7 @@
       <c r="D113" t="s">
         <v>274</v>
       </c>
-      <c r="E113" s="4" t="s">
+      <c r="E113" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14577,7 +14576,7 @@
       <c r="D114" t="s">
         <v>275</v>
       </c>
-      <c r="E114" s="4" t="s">
+      <c r="E114" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14594,7 +14593,7 @@
       <c r="D115" t="s">
         <v>276</v>
       </c>
-      <c r="E115" s="4" t="s">
+      <c r="E115" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14611,7 +14610,7 @@
       <c r="D116" t="s">
         <v>277</v>
       </c>
-      <c r="E116" s="4" t="s">
+      <c r="E116" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14628,7 +14627,7 @@
       <c r="D117" t="s">
         <v>278</v>
       </c>
-      <c r="E117" s="4" t="s">
+      <c r="E117" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14645,7 +14644,7 @@
       <c r="D118" t="s">
         <v>279</v>
       </c>
-      <c r="E118" s="4" t="s">
+      <c r="E118" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14662,7 +14661,7 @@
       <c r="D119" t="s">
         <v>280</v>
       </c>
-      <c r="E119" s="4" t="s">
+      <c r="E119" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14679,7 +14678,7 @@
       <c r="D120" t="s">
         <v>281</v>
       </c>
-      <c r="E120" s="4" t="s">
+      <c r="E120" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14696,7 +14695,7 @@
       <c r="D121" t="s">
         <v>282</v>
       </c>
-      <c r="E121" s="4" t="s">
+      <c r="E121" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14713,7 +14712,7 @@
       <c r="D122" t="s">
         <v>283</v>
       </c>
-      <c r="E122" s="4" t="s">
+      <c r="E122" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14730,7 +14729,7 @@
       <c r="D123" t="s">
         <v>284</v>
       </c>
-      <c r="E123" s="4" t="s">
+      <c r="E123" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14747,7 +14746,7 @@
       <c r="D124" t="s">
         <v>285</v>
       </c>
-      <c r="E124" s="4" t="s">
+      <c r="E124" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14764,7 +14763,7 @@
       <c r="D125" t="s">
         <v>286</v>
       </c>
-      <c r="E125" s="4" t="s">
+      <c r="E125" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14781,7 +14780,7 @@
       <c r="D126" t="s">
         <v>287</v>
       </c>
-      <c r="E126" s="4" t="s">
+      <c r="E126" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14798,7 +14797,7 @@
       <c r="D127" t="s">
         <v>288</v>
       </c>
-      <c r="E127" s="4" t="s">
+      <c r="E127" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14815,7 +14814,7 @@
       <c r="D128" t="s">
         <v>289</v>
       </c>
-      <c r="E128" s="4" t="s">
+      <c r="E128" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14832,7 +14831,7 @@
       <c r="D129" t="s">
         <v>290</v>
       </c>
-      <c r="E129" s="4" t="s">
+      <c r="E129" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14849,7 +14848,7 @@
       <c r="D130" t="s">
         <v>291</v>
       </c>
-      <c r="E130" s="4" t="s">
+      <c r="E130" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14866,7 +14865,7 @@
       <c r="D131" t="s">
         <v>292</v>
       </c>
-      <c r="E131" s="4" t="s">
+      <c r="E131" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14883,7 +14882,7 @@
       <c r="D132" t="s">
         <v>293</v>
       </c>
-      <c r="E132" s="4" t="s">
+      <c r="E132" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14900,7 +14899,7 @@
       <c r="D133" t="s">
         <v>294</v>
       </c>
-      <c r="E133" s="4" t="s">
+      <c r="E133" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14917,7 +14916,7 @@
       <c r="D134" t="s">
         <v>295</v>
       </c>
-      <c r="E134" s="4" t="s">
+      <c r="E134" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14934,7 +14933,7 @@
       <c r="D135" t="s">
         <v>296</v>
       </c>
-      <c r="E135" s="4" t="s">
+      <c r="E135" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14951,7 +14950,7 @@
       <c r="D136" t="s">
         <v>297</v>
       </c>
-      <c r="E136" s="4" t="s">
+      <c r="E136" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14968,7 +14967,7 @@
       <c r="D137" t="s">
         <v>298</v>
       </c>
-      <c r="E137" s="4" t="s">
+      <c r="E137" t="s">
         <v>96</v>
       </c>
     </row>
@@ -14985,7 +14984,7 @@
       <c r="D138" t="s">
         <v>299</v>
       </c>
-      <c r="E138" s="4" t="s">
+      <c r="E138" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15002,7 +15001,7 @@
       <c r="D139" t="s">
         <v>300</v>
       </c>
-      <c r="E139" s="4" t="s">
+      <c r="E139" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15019,7 +15018,7 @@
       <c r="D140" t="s">
         <v>301</v>
       </c>
-      <c r="E140" s="4" t="s">
+      <c r="E140" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15036,7 +15035,7 @@
       <c r="D141" t="s">
         <v>302</v>
       </c>
-      <c r="E141" s="4" t="s">
+      <c r="E141" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15053,7 +15052,7 @@
       <c r="D142" t="s">
         <v>303</v>
       </c>
-      <c r="E142" s="4" t="s">
+      <c r="E142" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15070,7 +15069,7 @@
       <c r="D143" t="s">
         <v>304</v>
       </c>
-      <c r="E143" s="4" t="s">
+      <c r="E143" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15087,7 +15086,7 @@
       <c r="D144" t="s">
         <v>305</v>
       </c>
-      <c r="E144" s="4" t="s">
+      <c r="E144" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15104,7 +15103,7 @@
       <c r="D145" t="s">
         <v>306</v>
       </c>
-      <c r="E145" s="4" t="s">
+      <c r="E145" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15121,7 +15120,7 @@
       <c r="D146" t="s">
         <v>307</v>
       </c>
-      <c r="E146" s="4" t="s">
+      <c r="E146" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15138,7 +15137,7 @@
       <c r="D147" t="s">
         <v>308</v>
       </c>
-      <c r="E147" s="4" t="s">
+      <c r="E147" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15155,7 +15154,7 @@
       <c r="D148" t="s">
         <v>309</v>
       </c>
-      <c r="E148" s="4" t="s">
+      <c r="E148" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15172,7 +15171,7 @@
       <c r="D149" t="s">
         <v>310</v>
       </c>
-      <c r="E149" s="4" t="s">
+      <c r="E149" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15189,7 +15188,7 @@
       <c r="D150" t="s">
         <v>311</v>
       </c>
-      <c r="E150" s="4" t="s">
+      <c r="E150" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15206,7 +15205,7 @@
       <c r="D151" t="s">
         <v>312</v>
       </c>
-      <c r="E151" s="4" t="s">
+      <c r="E151" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15223,7 +15222,7 @@
       <c r="D152" t="s">
         <v>313</v>
       </c>
-      <c r="E152" s="4" t="s">
+      <c r="E152" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15240,7 +15239,7 @@
       <c r="D153" t="s">
         <v>314</v>
       </c>
-      <c r="E153" s="4" t="s">
+      <c r="E153" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15257,7 +15256,7 @@
       <c r="D154" t="s">
         <v>315</v>
       </c>
-      <c r="E154" s="4" t="s">
+      <c r="E154" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15274,7 +15273,7 @@
       <c r="D155" t="s">
         <v>316</v>
       </c>
-      <c r="E155" s="4" t="s">
+      <c r="E155" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15291,7 +15290,7 @@
       <c r="D156" t="s">
         <v>317</v>
       </c>
-      <c r="E156" s="4" t="s">
+      <c r="E156" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15308,7 +15307,7 @@
       <c r="D157" t="s">
         <v>318</v>
       </c>
-      <c r="E157" s="4" t="s">
+      <c r="E157" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15325,7 +15324,7 @@
       <c r="D158" t="s">
         <v>319</v>
       </c>
-      <c r="E158" s="4" t="s">
+      <c r="E158" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15342,7 +15341,7 @@
       <c r="D159" t="s">
         <v>320</v>
       </c>
-      <c r="E159" s="4" t="s">
+      <c r="E159" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15359,7 +15358,7 @@
       <c r="D160" t="s">
         <v>321</v>
       </c>
-      <c r="E160" s="4" t="s">
+      <c r="E160" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15376,7 +15375,7 @@
       <c r="D161" t="s">
         <v>322</v>
       </c>
-      <c r="E161" s="4" t="s">
+      <c r="E161" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15393,7 +15392,7 @@
       <c r="D162" t="s">
         <v>323</v>
       </c>
-      <c r="E162" s="4" t="s">
+      <c r="E162" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15410,7 +15409,7 @@
       <c r="D163" t="s">
         <v>324</v>
       </c>
-      <c r="E163" s="4" t="s">
+      <c r="E163" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15427,7 +15426,7 @@
       <c r="D164" t="s">
         <v>325</v>
       </c>
-      <c r="E164" s="4" t="s">
+      <c r="E164" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15444,7 +15443,7 @@
       <c r="D165" t="s">
         <v>326</v>
       </c>
-      <c r="E165" s="4" t="s">
+      <c r="E165" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15461,7 +15460,7 @@
       <c r="D166" t="s">
         <v>327</v>
       </c>
-      <c r="E166" s="4" t="s">
+      <c r="E166" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15478,7 +15477,7 @@
       <c r="D167" t="s">
         <v>328</v>
       </c>
-      <c r="E167" s="4" t="s">
+      <c r="E167" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15495,7 +15494,7 @@
       <c r="D168" t="s">
         <v>329</v>
       </c>
-      <c r="E168" s="4" t="s">
+      <c r="E168" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15512,7 +15511,7 @@
       <c r="D169" t="s">
         <v>330</v>
       </c>
-      <c r="E169" s="4" t="s">
+      <c r="E169" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15529,7 +15528,7 @@
       <c r="D170" t="s">
         <v>331</v>
       </c>
-      <c r="E170" s="4" t="s">
+      <c r="E170" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15546,7 +15545,7 @@
       <c r="D171" t="s">
         <v>332</v>
       </c>
-      <c r="E171" s="4" t="s">
+      <c r="E171" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15563,7 +15562,7 @@
       <c r="D172" t="s">
         <v>333</v>
       </c>
-      <c r="E172" s="4" t="s">
+      <c r="E172" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15580,7 +15579,7 @@
       <c r="D173" t="s">
         <v>334</v>
       </c>
-      <c r="E173" s="4" t="s">
+      <c r="E173" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15597,7 +15596,7 @@
       <c r="D174" t="s">
         <v>335</v>
       </c>
-      <c r="E174" s="4" t="s">
+      <c r="E174" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15614,7 +15613,7 @@
       <c r="D175" t="s">
         <v>336</v>
       </c>
-      <c r="E175" s="4" t="s">
+      <c r="E175" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15631,7 +15630,7 @@
       <c r="D176" t="s">
         <v>337</v>
       </c>
-      <c r="E176" s="4" t="s">
+      <c r="E176" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15648,7 +15647,7 @@
       <c r="D177" t="s">
         <v>338</v>
       </c>
-      <c r="E177" s="4" t="s">
+      <c r="E177" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15665,7 +15664,7 @@
       <c r="D178" t="s">
         <v>339</v>
       </c>
-      <c r="E178" s="4" t="s">
+      <c r="E178" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15682,7 +15681,7 @@
       <c r="D179" t="s">
         <v>340</v>
       </c>
-      <c r="E179" s="4" t="s">
+      <c r="E179" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15699,7 +15698,7 @@
       <c r="D180" t="s">
         <v>341</v>
       </c>
-      <c r="E180" s="4" t="s">
+      <c r="E180" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15716,7 +15715,7 @@
       <c r="D181" t="s">
         <v>342</v>
       </c>
-      <c r="E181" s="4" t="s">
+      <c r="E181" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15733,7 +15732,7 @@
       <c r="D182" t="s">
         <v>343</v>
       </c>
-      <c r="E182" s="4" t="s">
+      <c r="E182" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15750,7 +15749,7 @@
       <c r="D183" t="s">
         <v>344</v>
       </c>
-      <c r="E183" s="4" t="s">
+      <c r="E183" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15767,7 +15766,7 @@
       <c r="D184" t="s">
         <v>345</v>
       </c>
-      <c r="E184" s="4" t="s">
+      <c r="E184" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15784,7 +15783,7 @@
       <c r="D185" t="s">
         <v>346</v>
       </c>
-      <c r="E185" s="4" t="s">
+      <c r="E185" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15801,7 +15800,7 @@
       <c r="D186" t="s">
         <v>347</v>
       </c>
-      <c r="E186" s="4" t="s">
+      <c r="E186" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15818,7 +15817,7 @@
       <c r="D187" t="s">
         <v>348</v>
       </c>
-      <c r="E187" s="4" t="s">
+      <c r="E187" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15835,7 +15834,7 @@
       <c r="D188" t="s">
         <v>349</v>
       </c>
-      <c r="E188" s="4" t="s">
+      <c r="E188" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15852,7 +15851,7 @@
       <c r="D189" t="s">
         <v>350</v>
       </c>
-      <c r="E189" s="4" t="s">
+      <c r="E189" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15869,7 +15868,7 @@
       <c r="D190" t="s">
         <v>351</v>
       </c>
-      <c r="E190" s="4" t="s">
+      <c r="E190" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15886,7 +15885,7 @@
       <c r="D191" t="s">
         <v>352</v>
       </c>
-      <c r="E191" s="4" t="s">
+      <c r="E191" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15903,7 +15902,7 @@
       <c r="D192" t="s">
         <v>542</v>
       </c>
-      <c r="E192" s="4" t="s">
+      <c r="E192" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15920,7 +15919,7 @@
       <c r="D193" t="s">
         <v>543</v>
       </c>
-      <c r="E193" s="4" t="s">
+      <c r="E193" t="s">
         <v>96</v>
       </c>
     </row>
@@ -15937,7 +15936,7 @@
       <c r="D194" t="s">
         <v>544</v>
       </c>
-      <c r="E194" s="4" t="s">
+      <c r="E194" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15954,7 +15953,7 @@
       <c r="D195" t="s">
         <v>545</v>
       </c>
-      <c r="E195" s="4" t="s">
+      <c r="E195" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15971,7 +15970,7 @@
       <c r="D196" t="s">
         <v>546</v>
       </c>
-      <c r="E196" s="4" t="s">
+      <c r="E196" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15988,7 +15987,7 @@
       <c r="D197" t="s">
         <v>547</v>
       </c>
-      <c r="E197" s="4" t="s">
+      <c r="E197" t="s">
         <v>91</v>
       </c>
     </row>
@@ -16005,7 +16004,7 @@
       <c r="D198" t="s">
         <v>548</v>
       </c>
-      <c r="E198" s="4" t="s">
+      <c r="E198" t="s">
         <v>91</v>
       </c>
     </row>
@@ -17669,7 +17668,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -17726,7 +17725,7 @@
         <v>44</v>
       </c>
       <c r="G2" s="1">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="H2">
         <v>0</v>

</xml_diff>